<commit_message>
fix(msg_references.csv): Header mislabel fixed
VehicleLocalPosition_delta_vx --> _delta_vxy_0
VehicleLocalPosition_delta_vy --> _delta_vxy_1
</commit_message>
<xml_diff>
--- a/msg_reference.xlsx
+++ b/msg_reference.xlsx
@@ -767,7 +767,7 @@
     <t xml:space="preserve">Down position (negative altitude) in NED earth-fixed frame</t>
   </si>
   <si>
-    <t xml:space="preserve">VehicleLocalPosition_delta_x</t>
+    <t xml:space="preserve">VehicleLocalPosition_delta_xy_0</t>
   </si>
   <si>
     <t xml:space="preserve">delta_xy_0</t>
@@ -776,7 +776,7 @@
     <t xml:space="preserve">Amount of lateral shift of position estimate in latest reset in x</t>
   </si>
   <si>
-    <t xml:space="preserve">VehicleLocalPosition_delta_y</t>
+    <t xml:space="preserve">VehicleLocalPosition_delta_xy_1</t>
   </si>
   <si>
     <t xml:space="preserve">delta_xy_1</t>
@@ -3076,7 +3076,7 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
@@ -3335,9 +3335,9 @@
   <dimension ref="A1:I347"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="D92" activeCellId="0" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>